<commit_message>
Tested after comment update.
Program works fine after comment update.
</commit_message>
<xml_diff>
--- a/utility_test/test.xlsx
+++ b/utility_test/test.xlsx
@@ -347,7 +347,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -355,7 +355,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:2" r="1">
       <c t="n" r="A1">
@@ -438,6 +438,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" top="1" left="0.75" header="0.5" footer="0.5"/>
+  <pageMargins top="1" header="0.5" left="0.75" right="0.75" bottom="1" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>